<commit_message>
Added model features: - "Choke" constraints for flows and elements - Plotting module for model outputs (generic) - Technology "enable_year" configuration
</commit_message>
<xml_diff>
--- a/data/interim_calc/passenger.xlsx
+++ b/data/interim_calc/passenger.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruiziv/switchdrive/ACCURACY/RESTORE/data/interim_calc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333A1791-6810-C441-A124-016DEDB0AB27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D9713B-883A-9446-8F0F-8AD6E02C9F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19900" activeTab="15" xr2:uid="{49D628A3-50CA-2542-B55B-8B6118BC3501}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19900" activeTab="5" xr2:uid="{49D628A3-50CA-2542-B55B-8B6118BC3501}"/>
   </bookViews>
   <sheets>
     <sheet name="Datasets" sheetId="26" r:id="rId1"/>
@@ -2194,10 +2194,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
@@ -21871,10 +21871,10 @@
   <dimension ref="A1:T49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="S40" sqref="S40:S46"/>
+      <selection pane="bottomRight" activeCell="W29" sqref="W29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25868,7 +25868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5927047-D280-F74C-B51D-AE1E014F3194}">
   <dimension ref="A1:CI51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
@@ -32480,7 +32480,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight" activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -40352,25 +40352,25 @@
       </c>
       <c r="C1" s="27"/>
       <c r="D1" s="47"/>
-      <c r="E1" s="103" t="s">
+      <c r="E1" s="104" t="s">
         <v>199</v>
       </c>
-      <c r="F1" s="103"/>
+      <c r="F1" s="104"/>
       <c r="G1" s="46"/>
-      <c r="H1" s="103" t="s">
+      <c r="H1" s="104" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="103"/>
+      <c r="I1" s="104"/>
       <c r="J1" s="46"/>
-      <c r="K1" s="103" t="s">
+      <c r="K1" s="104" t="s">
         <v>46</v>
       </c>
-      <c r="L1" s="103"/>
+      <c r="L1" s="104"/>
       <c r="M1" s="46"/>
-      <c r="N1" s="103" t="s">
+      <c r="N1" s="104" t="s">
         <v>31</v>
       </c>
-      <c r="O1" s="103"/>
+      <c r="O1" s="104"/>
       <c r="P1" s="6"/>
       <c r="Q1" s="59" t="s">
         <v>316</v>
@@ -40378,13 +40378,13 @@
       <c r="R1" s="59"/>
       <c r="S1" s="59"/>
       <c r="T1"/>
-      <c r="U1" s="104" t="s">
+      <c r="U1" s="103" t="s">
         <v>317</v>
       </c>
-      <c r="V1" s="104"/>
-      <c r="W1" s="104"/>
-      <c r="X1" s="104"/>
-      <c r="Y1" s="104"/>
+      <c r="V1" s="103"/>
+      <c r="W1" s="103"/>
+      <c r="X1" s="103"/>
+      <c r="Y1" s="103"/>
       <c r="Z1" s="48"/>
       <c r="AA1" s="26"/>
       <c r="AB1" s="58" t="s">
@@ -40404,20 +40404,20 @@
       <c r="AN1" s="60"/>
       <c r="AO1"/>
       <c r="AP1"/>
-      <c r="AQ1" s="104" t="s">
+      <c r="AQ1" s="103" t="s">
         <v>327</v>
       </c>
-      <c r="AR1" s="104"/>
-      <c r="AS1" s="104"/>
-      <c r="AT1" s="104"/>
-      <c r="AU1" s="104"/>
-      <c r="AV1" s="104"/>
-      <c r="AW1" s="104"/>
-      <c r="AX1" s="104"/>
-      <c r="AY1" s="104"/>
-      <c r="AZ1" s="104"/>
-      <c r="BA1" s="104"/>
-      <c r="BB1" s="104"/>
+      <c r="AR1" s="103"/>
+      <c r="AS1" s="103"/>
+      <c r="AT1" s="103"/>
+      <c r="AU1" s="103"/>
+      <c r="AV1" s="103"/>
+      <c r="AW1" s="103"/>
+      <c r="AX1" s="103"/>
+      <c r="AY1" s="103"/>
+      <c r="AZ1" s="103"/>
+      <c r="BA1" s="103"/>
+      <c r="BB1" s="103"/>
     </row>
     <row r="2" spans="1:54" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="56" t="s">
@@ -43879,10 +43879,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="AQ2:BB2"/>
-    <mergeCell ref="AQ1:BB1"/>
-    <mergeCell ref="AB2:AM2"/>
-    <mergeCell ref="E2:F2"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="AB1:AN1"/>
     <mergeCell ref="H2:I2"/>
@@ -43896,6 +43892,10 @@
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="U2:V2"/>
     <mergeCell ref="U1:Y1"/>
+    <mergeCell ref="AQ2:BB2"/>
+    <mergeCell ref="AQ1:BB1"/>
+    <mergeCell ref="AB2:AM2"/>
+    <mergeCell ref="E2:F2"/>
   </mergeCells>
   <conditionalFormatting sqref="H6:I38">
     <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
@@ -47362,10 +47362,10 @@
   <dimension ref="A1:CB45"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="U7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="Y6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AI37" sqref="AI37"/>
+      <selection pane="bottomRight" activeCell="AO7" sqref="AO7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -53920,7 +53920,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="N40" sqref="N40"/>
+      <selection pane="bottomRight" activeCell="N5" sqref="N5:N37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -62888,11 +62888,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EB7D03A-22B7-4641-ACF5-FC3E5BEB015D}">
   <dimension ref="A1:AR48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="H17" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="X27" sqref="X27"/>
+      <selection pane="bottomRight" activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -67543,7 +67543,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="I44" sqref="I44"/>
+      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>